<commit_message>
ABM-API Guias y API Noticias
</commit_message>
<xml_diff>
--- a/Docs/Documentos Turismo/SENDERISMO Y TREKKING SAN JUAN - (SENDEROS PARA APP FIESTA DEL SOL 2018).xlsx
+++ b/Docs/Documentos Turismo/SENDERISMO Y TREKKING SAN JUAN - (SENDEROS PARA APP FIESTA DEL SOL 2018).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SENDEROS APP" sheetId="1" r:id="rId1"/>
@@ -3335,7 +3335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="173">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -3717,6 +3717,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4023,7 +4029,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
@@ -5574,8 +5580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5588,18 +5594,18 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="87" t="s">
+    <row r="3" spans="1:1" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="173" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="88" t="s">
+    <row r="4" spans="1:1" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="174" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="88" t="s">
+    <row r="5" spans="1:1" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="174" t="s">
         <v>98</v>
       </c>
     </row>

</xml_diff>